<commit_message>
Periodic backup of files.
</commit_message>
<xml_diff>
--- a/X-Project tools/Excel/Bower Cheatsheet.xlsx
+++ b/X-Project tools/Excel/Bower Cheatsheet.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
-    <sheet name="node.js cheatsheet" sheetId="4" r:id="rId1"/>
+    <sheet name="Bower cheatsheet" sheetId="4" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Installs an npm package in the global local registry from a tarball file.</t>
   </si>
@@ -72,12 +72,15 @@
   <si>
     <t>Fetchs current artifact dependencies from remote repositories.</t>
   </si>
+  <si>
+    <t>bower cache clean</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -326,12 +329,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -405,7 +411,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -440,7 +445,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -616,17 +620,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B1:AF36"/>
+  <dimension ref="B1:AF37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="AB6" sqref="AB6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="26" width="2.85546875" customWidth="1"/>
     <col min="27" max="27" width="15" customWidth="1" outlineLevel="1"/>
@@ -637,7 +641,7 @@
     <col min="32" max="32" width="46" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:32">
       <c r="B1" s="16" t="s">
         <v>6</v>
       </c>
@@ -678,7 +682,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:32">
       <c r="B2" s="17" t="s">
         <v>15</v>
       </c>
@@ -715,7 +719,7 @@
       </c>
       <c r="AF2" s="7"/>
     </row>
-    <row r="3" spans="2:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:32" ht="30">
       <c r="B3" s="17" t="s">
         <v>16</v>
       </c>
@@ -752,44 +756,43 @@
       </c>
       <c r="AF3" s="7"/>
     </row>
-    <row r="4" spans="2:32" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="12"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
-      <c r="V4" s="10"/>
-      <c r="W4" s="10"/>
-      <c r="X4" s="10"/>
-      <c r="Y4" s="10"/>
-      <c r="Z4" s="11"/>
+    <row r="4" spans="2:32">
+      <c r="B4" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="18"/>
+      <c r="Q4" s="18"/>
+      <c r="R4" s="18"/>
+      <c r="S4" s="18"/>
+      <c r="T4" s="18"/>
+      <c r="U4" s="18"/>
+      <c r="V4" s="18"/>
+      <c r="W4" s="18"/>
+      <c r="X4" s="18"/>
+      <c r="Y4" s="18"/>
+      <c r="Z4" s="19"/>
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
       <c r="AC4" s="2"/>
       <c r="AD4" s="2"/>
-      <c r="AE4" s="1"/>
-      <c r="AF4" s="6"/>
-    </row>
-    <row r="5" spans="2:32" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="12" t="str">
-        <f>"npm install "&amp;AB5&amp;" -g"</f>
-        <v>npm install tsb-generator-commons-0.1.2.tgz -g</v>
-      </c>
+      <c r="AE4" s="8"/>
+      <c r="AF4" s="7"/>
+    </row>
+    <row r="5" spans="2:32" collapsed="1">
+      <c r="B5" s="12"/>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
@@ -814,22 +817,17 @@
       <c r="X5" s="10"/>
       <c r="Y5" s="10"/>
       <c r="Z5" s="11"/>
-      <c r="AA5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB5" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="AA5" s="2"/>
+      <c r="AB5" s="2"/>
       <c r="AC5" s="2"/>
       <c r="AD5" s="2"/>
-      <c r="AE5" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="AE5" s="1"/>
       <c r="AF5" s="6"/>
     </row>
-    <row r="6" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B6" s="12" t="s">
-        <v>7</v>
+    <row r="6" spans="2:32" ht="30">
+      <c r="B6" s="12" t="str">
+        <f>"npm install "&amp;AB6&amp;" -g"</f>
+        <v>npm install tsb-generator-commons-0.1.2.tgz -g</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
@@ -855,20 +853,24 @@
       <c r="X6" s="10"/>
       <c r="Y6" s="10"/>
       <c r="Z6" s="11"/>
-      <c r="AA6" s="2"/>
-      <c r="AB6" s="2"/>
+      <c r="AA6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB6" s="5" t="s">
+        <v>1</v>
+      </c>
       <c r="AC6" s="2"/>
       <c r="AD6" s="2"/>
       <c r="AE6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AF6" s="1"/>
-    </row>
-    <row r="7" spans="2:32" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="3"/>
-      <c r="C7" s="10" t="s">
-        <v>9</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="AF6" s="6"/>
+    </row>
+    <row r="7" spans="2:32">
+      <c r="B7" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="10"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
@@ -897,14 +899,14 @@
       <c r="AC7" s="2"/>
       <c r="AD7" s="2"/>
       <c r="AE7" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="AF7" s="1"/>
     </row>
-    <row r="8" spans="2:32" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:32" outlineLevel="1">
       <c r="B8" s="3"/>
       <c r="C8" s="10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
@@ -934,14 +936,14 @@
       <c r="AC8" s="2"/>
       <c r="AD8" s="2"/>
       <c r="AE8" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AF8" s="1"/>
     </row>
-    <row r="9" spans="2:32" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:32" outlineLevel="1">
       <c r="B9" s="3"/>
       <c r="C9" s="10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
@@ -971,13 +973,15 @@
       <c r="AC9" s="2"/>
       <c r="AD9" s="2"/>
       <c r="AE9" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="AF9" s="1"/>
     </row>
-    <row r="10" spans="2:32" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:32" ht="30" outlineLevel="1">
       <c r="B10" s="3"/>
-      <c r="C10" s="10"/>
+      <c r="C10" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
@@ -1005,11 +1009,13 @@
       <c r="AB10" s="2"/>
       <c r="AC10" s="2"/>
       <c r="AD10" s="2"/>
-      <c r="AE10" s="1"/>
+      <c r="AE10" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="AF10" s="1"/>
     </row>
-    <row r="11" spans="2:32" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="12"/>
+    <row r="11" spans="2:32" outlineLevel="1">
+      <c r="B11" s="3"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
@@ -1041,7 +1047,7 @@
       <c r="AE11" s="1"/>
       <c r="AF11" s="1"/>
     </row>
-    <row r="12" spans="2:32" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:32" collapsed="1">
       <c r="B12" s="12"/>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
@@ -1074,7 +1080,7 @@
       <c r="AE12" s="1"/>
       <c r="AF12" s="1"/>
     </row>
-    <row r="13" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:32" collapsed="1">
       <c r="B13" s="12"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
@@ -1107,7 +1113,7 @@
       <c r="AE13" s="1"/>
       <c r="AF13" s="1"/>
     </row>
-    <row r="14" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:32">
       <c r="B14" s="12"/>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
@@ -1140,7 +1146,7 @@
       <c r="AE14" s="1"/>
       <c r="AF14" s="1"/>
     </row>
-    <row r="15" spans="2:32" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:32">
       <c r="B15" s="12"/>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
@@ -1173,8 +1179,8 @@
       <c r="AE15" s="1"/>
       <c r="AF15" s="1"/>
     </row>
-    <row r="16" spans="2:32" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="3"/>
+    <row r="16" spans="2:32" collapsed="1">
+      <c r="B16" s="12"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
@@ -1206,7 +1212,7 @@
       <c r="AE16" s="1"/>
       <c r="AF16" s="1"/>
     </row>
-    <row r="17" spans="2:32" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:32" hidden="1" outlineLevel="1">
       <c r="B17" s="3"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
@@ -1239,9 +1245,9 @@
       <c r="AE17" s="1"/>
       <c r="AF17" s="1"/>
     </row>
-    <row r="18" spans="2:32" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:32" hidden="1" outlineLevel="1">
       <c r="B18" s="3"/>
-      <c r="C18" s="4"/>
+      <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
@@ -1272,7 +1278,7 @@
       <c r="AE18" s="1"/>
       <c r="AF18" s="1"/>
     </row>
-    <row r="19" spans="2:32" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:32" hidden="1" outlineLevel="2">
       <c r="B19" s="3"/>
       <c r="C19" s="4"/>
       <c r="D19" s="10"/>
@@ -1305,10 +1311,10 @@
       <c r="AE19" s="1"/>
       <c r="AF19" s="1"/>
     </row>
-    <row r="20" spans="2:32" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:32" hidden="1" outlineLevel="2">
       <c r="B20" s="3"/>
       <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
+      <c r="D20" s="10"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
@@ -1338,7 +1344,7 @@
       <c r="AE20" s="1"/>
       <c r="AF20" s="1"/>
     </row>
-    <row r="21" spans="2:32" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:32" hidden="1" outlineLevel="3">
       <c r="B21" s="3"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
@@ -1371,11 +1377,11 @@
       <c r="AE21" s="1"/>
       <c r="AF21" s="1"/>
     </row>
-    <row r="22" spans="2:32" hidden="1" outlineLevel="4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:32" hidden="1" outlineLevel="3">
       <c r="B22" s="3"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
+      <c r="E22" s="10"/>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
@@ -1404,7 +1410,7 @@
       <c r="AE22" s="1"/>
       <c r="AF22" s="1"/>
     </row>
-    <row r="23" spans="2:32" hidden="1" outlineLevel="4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:32" hidden="1" outlineLevel="4">
       <c r="B23" s="3"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -1437,12 +1443,12 @@
       <c r="AE23" s="1"/>
       <c r="AF23" s="1"/>
     </row>
-    <row r="24" spans="2:32" hidden="1" outlineLevel="5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:32" hidden="1" outlineLevel="4">
       <c r="B24" s="3"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
+      <c r="F24" s="10"/>
       <c r="G24" s="10"/>
       <c r="H24" s="10"/>
       <c r="I24" s="10"/>
@@ -1463,10 +1469,14 @@
       <c r="X24" s="10"/>
       <c r="Y24" s="10"/>
       <c r="Z24" s="11"/>
+      <c r="AA24" s="2"/>
+      <c r="AB24" s="2"/>
+      <c r="AC24" s="2"/>
+      <c r="AD24" s="2"/>
       <c r="AE24" s="1"/>
       <c r="AF24" s="1"/>
     </row>
-    <row r="25" spans="2:32" hidden="1" outlineLevel="5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:32" hidden="1" outlineLevel="5">
       <c r="B25" s="3"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -1495,13 +1505,13 @@
       <c r="AE25" s="1"/>
       <c r="AF25" s="1"/>
     </row>
-    <row r="26" spans="2:32" hidden="1" outlineLevel="6" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:32" hidden="1" outlineLevel="5">
       <c r="B26" s="3"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
+      <c r="G26" s="10"/>
       <c r="H26" s="10"/>
       <c r="I26" s="10"/>
       <c r="J26" s="10"/>
@@ -1524,7 +1534,7 @@
       <c r="AE26" s="1"/>
       <c r="AF26" s="1"/>
     </row>
-    <row r="27" spans="2:32" hidden="1" outlineLevel="6" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:32" hidden="1" outlineLevel="6">
       <c r="B27" s="3"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
@@ -1553,14 +1563,14 @@
       <c r="AE27" s="1"/>
       <c r="AF27" s="1"/>
     </row>
-    <row r="28" spans="2:32" hidden="1" outlineLevel="7" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:32" hidden="1" outlineLevel="6">
       <c r="B28" s="3"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
+      <c r="H28" s="10"/>
       <c r="I28" s="10"/>
       <c r="J28" s="10"/>
       <c r="K28" s="10"/>
@@ -1582,7 +1592,7 @@
       <c r="AE28" s="1"/>
       <c r="AF28" s="1"/>
     </row>
-    <row r="29" spans="2:32" hidden="1" outlineLevel="7" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:32" hidden="1" outlineLevel="7">
       <c r="B29" s="3"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -1611,14 +1621,14 @@
       <c r="AE29" s="1"/>
       <c r="AF29" s="1"/>
     </row>
-    <row r="30" spans="2:32" hidden="1" outlineLevel="6" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:32" hidden="1" outlineLevel="7">
       <c r="B30" s="3"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
-      <c r="H30" s="10"/>
+      <c r="H30" s="4"/>
       <c r="I30" s="10"/>
       <c r="J30" s="10"/>
       <c r="K30" s="10"/>
@@ -1640,13 +1650,13 @@
       <c r="AE30" s="1"/>
       <c r="AF30" s="1"/>
     </row>
-    <row r="31" spans="2:32" hidden="1" outlineLevel="5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:32" hidden="1" outlineLevel="6">
       <c r="B31" s="3"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
-      <c r="G31" s="10"/>
+      <c r="G31" s="4"/>
       <c r="H31" s="10"/>
       <c r="I31" s="10"/>
       <c r="J31" s="10"/>
@@ -1669,12 +1679,12 @@
       <c r="AE31" s="1"/>
       <c r="AF31" s="1"/>
     </row>
-    <row r="32" spans="2:32" hidden="1" outlineLevel="4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:32" hidden="1" outlineLevel="5">
       <c r="B32" s="3"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
-      <c r="F32" s="10"/>
+      <c r="F32" s="4"/>
       <c r="G32" s="10"/>
       <c r="H32" s="10"/>
       <c r="I32" s="10"/>
@@ -1698,11 +1708,11 @@
       <c r="AE32" s="1"/>
       <c r="AF32" s="1"/>
     </row>
-    <row r="33" spans="2:32" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:32" hidden="1" outlineLevel="4">
       <c r="B33" s="3"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
-      <c r="E33" s="10"/>
+      <c r="E33" s="4"/>
       <c r="F33" s="10"/>
       <c r="G33" s="10"/>
       <c r="H33" s="10"/>
@@ -1727,10 +1737,10 @@
       <c r="AE33" s="1"/>
       <c r="AF33" s="1"/>
     </row>
-    <row r="34" spans="2:32" hidden="1" outlineLevel="3" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:32" hidden="1" outlineLevel="3">
       <c r="B34" s="3"/>
       <c r="C34" s="4"/>
-      <c r="D34" s="10"/>
+      <c r="D34" s="4"/>
       <c r="E34" s="10"/>
       <c r="F34" s="10"/>
       <c r="G34" s="10"/>
@@ -1756,9 +1766,9 @@
       <c r="AE34" s="1"/>
       <c r="AF34" s="1"/>
     </row>
-    <row r="35" spans="2:32" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:32" hidden="1" outlineLevel="3">
       <c r="B35" s="3"/>
-      <c r="C35" s="10"/>
+      <c r="C35" s="4"/>
       <c r="D35" s="10"/>
       <c r="E35" s="10"/>
       <c r="F35" s="10"/>
@@ -1785,8 +1795,8 @@
       <c r="AE35" s="1"/>
       <c r="AF35" s="1"/>
     </row>
-    <row r="36" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B36" s="12"/>
+    <row r="36" spans="2:32" hidden="1" outlineLevel="2">
+      <c r="B36" s="3"/>
       <c r="C36" s="10"/>
       <c r="D36" s="10"/>
       <c r="E36" s="10"/>
@@ -1811,52 +1821,82 @@
       <c r="X36" s="10"/>
       <c r="Y36" s="10"/>
       <c r="Z36" s="11"/>
-      <c r="AA36" s="2"/>
-      <c r="AB36" s="2"/>
-      <c r="AC36" s="2"/>
-      <c r="AD36" s="2"/>
       <c r="AE36" s="1"/>
       <c r="AF36" s="1"/>
     </row>
+    <row r="37" spans="2:32">
+      <c r="B37" s="12"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="10"/>
+      <c r="K37" s="10"/>
+      <c r="L37" s="10"/>
+      <c r="M37" s="10"/>
+      <c r="N37" s="10"/>
+      <c r="O37" s="10"/>
+      <c r="P37" s="10"/>
+      <c r="Q37" s="10"/>
+      <c r="R37" s="10"/>
+      <c r="S37" s="10"/>
+      <c r="T37" s="10"/>
+      <c r="U37" s="10"/>
+      <c r="V37" s="10"/>
+      <c r="W37" s="10"/>
+      <c r="X37" s="10"/>
+      <c r="Y37" s="10"/>
+      <c r="Z37" s="11"/>
+      <c r="AA37" s="2"/>
+      <c r="AB37" s="2"/>
+      <c r="AC37" s="2"/>
+      <c r="AD37" s="2"/>
+      <c r="AE37" s="1"/>
+      <c r="AF37" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="37">
-    <mergeCell ref="B6:Z6"/>
+  <mergeCells count="38">
+    <mergeCell ref="B7:Z7"/>
     <mergeCell ref="AA1:AD1"/>
     <mergeCell ref="B1:Z1"/>
     <mergeCell ref="B2:Z2"/>
+    <mergeCell ref="B6:Z6"/>
+    <mergeCell ref="B3:Z3"/>
     <mergeCell ref="B5:Z5"/>
-    <mergeCell ref="B3:Z3"/>
     <mergeCell ref="B4:Z4"/>
-    <mergeCell ref="C7:Z7"/>
     <mergeCell ref="C8:Z8"/>
+    <mergeCell ref="C9:Z9"/>
+    <mergeCell ref="B13:Z13"/>
+    <mergeCell ref="C11:Z11"/>
+    <mergeCell ref="C10:Z10"/>
     <mergeCell ref="B12:Z12"/>
-    <mergeCell ref="C10:Z10"/>
-    <mergeCell ref="C9:Z9"/>
-    <mergeCell ref="G24:Z24"/>
-    <mergeCell ref="B13:Z13"/>
+    <mergeCell ref="G25:Z25"/>
     <mergeCell ref="B14:Z14"/>
     <mergeCell ref="B15:Z15"/>
-    <mergeCell ref="C16:Z16"/>
+    <mergeCell ref="B16:Z16"/>
     <mergeCell ref="C17:Z17"/>
+    <mergeCell ref="C18:Z18"/>
+    <mergeCell ref="F24:Z24"/>
+    <mergeCell ref="D19:Z19"/>
+    <mergeCell ref="D20:Z20"/>
+    <mergeCell ref="E21:Z21"/>
+    <mergeCell ref="E22:Z22"/>
     <mergeCell ref="F23:Z23"/>
-    <mergeCell ref="B11:Z11"/>
-    <mergeCell ref="D18:Z18"/>
-    <mergeCell ref="D19:Z19"/>
-    <mergeCell ref="E20:Z20"/>
-    <mergeCell ref="E21:Z21"/>
-    <mergeCell ref="F22:Z22"/>
-    <mergeCell ref="D34:Z34"/>
-    <mergeCell ref="C35:Z35"/>
-    <mergeCell ref="B36:Z36"/>
-    <mergeCell ref="G25:Z25"/>
-    <mergeCell ref="H26:Z26"/>
+    <mergeCell ref="D35:Z35"/>
+    <mergeCell ref="C36:Z36"/>
+    <mergeCell ref="B37:Z37"/>
+    <mergeCell ref="G26:Z26"/>
     <mergeCell ref="H27:Z27"/>
-    <mergeCell ref="I28:Z28"/>
+    <mergeCell ref="H28:Z28"/>
     <mergeCell ref="I29:Z29"/>
-    <mergeCell ref="H30:Z30"/>
-    <mergeCell ref="G31:Z31"/>
-    <mergeCell ref="F32:Z32"/>
-    <mergeCell ref="E33:Z33"/>
+    <mergeCell ref="I30:Z30"/>
+    <mergeCell ref="H31:Z31"/>
+    <mergeCell ref="G32:Z32"/>
+    <mergeCell ref="F33:Z33"/>
+    <mergeCell ref="E34:Z34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>